<commit_message>
Changes on data file
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcos Manrique\IdeaProjects\ALKU_EW\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC72F0D3-BC8D-46C7-9BDC-6473EEA364B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB5F13F-358E-4B82-8432-E84BCBCB5FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{F69D7EBA-55A4-4DB3-A0F0-120D15E36C89}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{F69D7EBA-55A4-4DB3-A0F0-120D15E36C89}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,6 @@
     <sheet name="AA" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -179,15 +178,9 @@
     <t>Candidate_FirstName</t>
   </si>
   <si>
-    <t>Ajay</t>
-  </si>
-  <si>
     <t>Candidate_LastName</t>
   </si>
   <si>
-    <t>Inampudi</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -372,6 +365,12 @@
   </si>
   <si>
     <t>Kronos WFC/WFD Developer</t>
+  </si>
+  <si>
+    <t>Donthula</t>
+  </si>
+  <si>
+    <t>Amruth</t>
   </si>
 </sst>
 </file>
@@ -769,7 +768,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -840,7 +839,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1039,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA41EC5-FA86-4139-95F4-8E346B58CD6F}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1071,7 +1070,7 @@
         <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -1091,10 +1090,10 @@
         <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1128,7 +1127,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
         <v>39</v>
@@ -1145,10 +1144,10 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1160,7 +1159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C4111E-4D69-43AE-8BDC-34DF9DAF71C7}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1187,40 +1186,40 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E1" t="s">
         <v>39</v>
       </c>
       <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
         <v>52</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>54</v>
-      </c>
-      <c r="H1" t="s">
-        <v>56</v>
       </c>
       <c r="I1" t="s">
         <v>43</v>
       </c>
       <c r="J1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" t="s">
         <v>58</v>
       </c>
-      <c r="L1" t="s">
-        <v>60</v>
-      </c>
       <c r="M1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
@@ -1234,24 +1233,24 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
         <v>51</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>53</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>55</v>
-      </c>
-      <c r="H2" t="s">
-        <v>57</v>
       </c>
       <c r="K2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
@@ -1265,30 +1264,30 @@
         <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" t="s">
         <v>99</v>
       </c>
-      <c r="F3" t="s">
+      <c r="J3" t="s">
         <v>100</v>
-      </c>
-      <c r="G3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" t="s">
-        <v>101</v>
-      </c>
-      <c r="J3" t="s">
-        <v>102</v>
       </c>
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
@@ -1302,30 +1301,30 @@
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" t="s">
         <v>94</v>
       </c>
-      <c r="F4" t="s">
+      <c r="J4" t="s">
         <v>95</v>
-      </c>
-      <c r="G4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I4" t="s">
-        <v>96</v>
-      </c>
-      <c r="J4" t="s">
-        <v>97</v>
       </c>
       <c r="K4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
@@ -1333,30 +1332,30 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" t="s">
         <v>55</v>
-      </c>
-      <c r="H5" t="s">
-        <v>57</v>
       </c>
       <c r="K5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
@@ -1364,32 +1363,32 @@
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
         <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" t="s">
         <v>55</v>
       </c>
-      <c r="H6" t="s">
+      <c r="K6" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="M6" s="3"/>
       <c r="N6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
@@ -1397,35 +1396,35 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
         <v>27</v>
       </c>
       <c r="D7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" t="s">
         <v>106</v>
       </c>
-      <c r="E7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F7" t="s">
-        <v>108</v>
-      </c>
       <c r="G7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" t="s">
         <v>55</v>
-      </c>
-      <c r="H7" t="s">
-        <v>57</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
@@ -1433,28 +1432,28 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" t="s">
         <v>55</v>
       </c>
-      <c r="H8" t="s">
-        <v>57</v>
-      </c>
       <c r="N8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
@@ -1462,28 +1461,28 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
       </c>
       <c r="D9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" t="s">
         <v>91</v>
       </c>
-      <c r="E9" t="s">
-        <v>93</v>
-      </c>
       <c r="F9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" t="s">
         <v>55</v>
       </c>
-      <c r="H9" t="s">
-        <v>57</v>
-      </c>
       <c r="N9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1529,7 +1528,7 @@
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1650,16 +1649,16 @@
         <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1673,19 +1672,19 @@
         <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change on Jobs candidate
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcos Manrique\IdeaProjects\ALKU_EW\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcos Manrique\Desktop\ALKU_EW\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB5F13F-358E-4B82-8432-E84BCBCB5FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C3A8A2-9B29-40B9-BFD3-658119E3F65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{F69D7EBA-55A4-4DB3-A0F0-120D15E36C89}"/>
   </bookViews>
@@ -367,10 +367,10 @@
     <t>Kronos WFC/WFD Developer</t>
   </si>
   <si>
-    <t>Donthula</t>
-  </si>
-  <si>
-    <t>Amruth</t>
+    <t>Ajay</t>
+  </si>
+  <si>
+    <t>Inampudi</t>
   </si>
 </sst>
 </file>
@@ -1039,7 +1039,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1090,10 +1090,10 @@
         <v>42</v>
       </c>
       <c r="F2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" t="s">
         <v>108</v>
-      </c>
-      <c r="G2" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>